<commit_message>
Final Changes - 22 June 2023
</commit_message>
<xml_diff>
--- a/TestData/T2245_Contacts_DuplicateManagement_AddNewDuplicateEmployeeFromContactsTab.xlsx
+++ b/TestData/T2245_Contacts_DuplicateManagement_AddNewDuplicateEmployeeFromContactsTab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E991ACE-25D5-46B6-B731-6E7A7F820FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55594D3-5183-4398-B814-1A1E8E23E9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Sonika Goyal</t>
   </si>
   <si>
-    <t>StandardTestCompany</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Test Houlihan</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
   </si>
 </sst>
 </file>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -570,19 +570,19 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -696,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>